<commit_message>
terminando con los procedimientos del sistema
</commit_message>
<xml_diff>
--- a/OLDinventario.xlsx
+++ b/OLDinventario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\inventario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B0A658-EC8B-47A6-863F-110812A556BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD3CB74-639D-4E22-B98A-4BBB09E4BB92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{9FA05147-BDF8-4DD5-8DCA-13E46F8E9F7B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{9FA05147-BDF8-4DD5-8DCA-13E46F8E9F7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Stock" sheetId="1" r:id="rId1"/>
@@ -6782,8 +6782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05E44D0F-81BA-4A89-89F8-49F572A4631A}">
   <dimension ref="B2:H931"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -29015,7 +29015,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CC50238-738D-44C4-9281-9594B7374CDB}">
   <dimension ref="B2:I944"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>

</xml_diff>